<commit_message>
implèmentation de <ajouter une ecole>
</commit_message>
<xml_diff>
--- a/uploads/imara.xlsx
+++ b/uploads/imara.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIMA\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C7268A-7377-4049-8B05-9736D5FF1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C01B3-3C5F-4E0F-990E-D30F52D65E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>imara</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
     <t>haut-katanga</t>
   </si>
   <si>
@@ -70,6 +67,108 @@
   </si>
   <si>
     <t>Sixième B</t>
+  </si>
+  <si>
+    <t>ntonda lobe wighens 1234</t>
+  </si>
+  <si>
+    <t>munga mangili cecil 1234</t>
+  </si>
+  <si>
+    <t>kayembe malamu alvine 1234</t>
+  </si>
+  <si>
+    <t>kalanga muwaya jeanne 1234</t>
+  </si>
+  <si>
+    <t>ilonga magbau aggee 1234</t>
+  </si>
+  <si>
+    <t>kazi mubere orbut 1234</t>
+  </si>
+  <si>
+    <t>batingala josué josué 1234</t>
+  </si>
+  <si>
+    <t>kabila kabila blessing 1234</t>
+  </si>
+  <si>
+    <t>mulumba kabobola dassaint 1234</t>
+  </si>
+  <si>
+    <t>ndala ndala daniel 1234</t>
+  </si>
+  <si>
+    <t>mumba mumba rolly 1234</t>
+  </si>
+  <si>
+    <t>tshola mwewa dorcas 1234</t>
+  </si>
+  <si>
+    <t>banza banza ken</t>
+  </si>
+  <si>
+    <t>ilunga ilunga daniel</t>
+  </si>
+  <si>
+    <t>mukebo kalasa ruth</t>
+  </si>
+  <si>
+    <t>ngoie mwambe ruth</t>
+  </si>
+  <si>
+    <t>ngoie mwane honorine</t>
+  </si>
+  <si>
+    <t>munga mangili cecil</t>
+  </si>
+  <si>
+    <t>mwandi mwadi deo</t>
+  </si>
+  <si>
+    <t>ntundu mumba dedorah</t>
+  </si>
+  <si>
+    <t>irung irung skot</t>
+  </si>
+  <si>
+    <t>kalanga muwaya jeanne</t>
+  </si>
+  <si>
+    <t>kalumba kikonde jean</t>
+  </si>
+  <si>
+    <t>kisuyu mukeba jenovic</t>
+  </si>
+  <si>
+    <t>kipasa kipasa gad</t>
+  </si>
+  <si>
+    <t>kolesha tshikashama dady</t>
+  </si>
+  <si>
+    <t>nzeba nzeba allegra</t>
+  </si>
+  <si>
+    <t>kafand kafand paul</t>
+  </si>
+  <si>
+    <t>kuluba kuluba gloria</t>
+  </si>
+  <si>
+    <t>sykiaba sykiaba lambert</t>
+  </si>
+  <si>
+    <t>ilunga nseya allegresse</t>
+  </si>
+  <si>
+    <t>ilunga kisha julie</t>
+  </si>
+  <si>
+    <t>ilunga kibemba polie</t>
+  </si>
+  <si>
+    <t>ssertzet</t>
   </si>
 </sst>
 </file>
@@ -107,7 +206,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -390,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,47 +515,166 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>70012</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
         <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>